<commit_message>
added more switch types e.g XOR and XNOR
</commit_message>
<xml_diff>
--- a/darkworld/model/data/floor builder World2.xlsx
+++ b/darkworld/model/data/floor builder World2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\DarkWorld\darkworld\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7E6D6C-446C-47C2-A461-934BCE74538E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194C48AD-770A-441B-9850-A162DBFD9B63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11685" yWindow="2295" windowWidth="28800" windowHeight="15840" tabRatio="904" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="3210" windowWidth="20910" windowHeight="15840" tabRatio="904" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blank" sheetId="49" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4484" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4482" uniqueCount="58">
   <si>
     <t>width</t>
   </si>
@@ -600,6 +600,18 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -4797,22 +4809,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="16" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6540,22 +6552,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="12" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8983,12 +8995,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15969,8 +15981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743F0388-C5FF-43B0-98FA-CAD5E57A342F}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19452,7 +19464,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19543,7 +19555,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -19555,7 +19567,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>5</v>
@@ -19570,7 +19582,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>48</v>
@@ -19606,11 +19618,11 @@
       <c r="Y2" s="7"/>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v xml:space="preserve">:          :        </v>
+        <v xml:space="preserve">:X   ?    x:        </v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB25" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>':          :        ',</v>
+        <v>':X   ?    x:        ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -20017,7 +20029,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>5</v>
@@ -20056,11 +20068,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">         ?          </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'         ?          ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -21166,22 +21178,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21194,8 +21206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BF4396-7159-40E9-8585-9EBFFD78FF01}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21447,12 +21459,8 @@
       <c r="E4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="12" t="s">
         <v>5</v>
       </c>
@@ -21499,11 +21507,11 @@
       <c r="Y4" s="7"/>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> fff    fff         </v>
+        <v xml:space="preserve"> fff  fff         </v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>' fff    fff         ',</v>
+        <v>' fff  fff         ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -21610,7 +21618,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>5</v>
@@ -21649,11 +21657,11 @@
       <c r="Y6" s="7"/>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  f      f          </v>
+        <v xml:space="preserve">  f      .          </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'  f      f          ',</v>
+        <v>'  f      .          ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -21685,7 +21693,7 @@
         <v>5</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>5</v>
@@ -21724,11 +21732,11 @@
       <c r="Y7" s="7"/>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  _                 </v>
+        <v xml:space="preserve">  _      .          </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'  _                 ',</v>
+        <v>'  _      .          ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -21760,7 +21768,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>5</v>
@@ -21799,11 +21807,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">         .          </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'         .          ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -22909,22 +22917,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>